<commit_message>
Add subcategory step implementation
</commit_message>
<xml_diff>
--- a/parametros/Datos.xlsx
+++ b/parametros/Datos.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semillero QA\ClickShopAutomation\parametros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semillero QA\projects\clickShop-automation\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567829FC-3CB6-44FB-8E49-EAD788555FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F40A3D2-767D-4F18-8682-57B70F8F3FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="AgregarProducto" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,11 +24,30 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Subcategoria</t>
+  </si>
+  <si>
+    <t>Vinos y licores</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -55,8 +74,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,14 +362,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update steps and add producto implementation
</commit_message>
<xml_diff>
--- a/parametros/Datos.xlsx
+++ b/parametros/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semillero QA\projects\clickShop-automation\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F40A3D2-767D-4F18-8682-57B70F8F3FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1889235C-288F-4C98-BC63-EBD1BB819A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,19 +25,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Subcategoria</t>
   </si>
   <si>
     <t>Vinos y licores</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>Cerveza Club Colombia Dorada lata x6und x330ml c-u</t>
+  </si>
+  <si>
+    <t>CorreoAsociarCompra</t>
+  </si>
+  <si>
+    <t>paangudi3@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,6 +61,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,10 +91,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -82,8 +103,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -362,29 +387,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{DE1D0565-2AFF-4F68-8106-A4E3B3E0AE08}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create steps and modal producto
</commit_message>
<xml_diff>
--- a/parametros/Datos.xlsx
+++ b/parametros/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semillero QA\projects\clickShop-automation\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1889235C-288F-4C98-BC63-EBD1BB819A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF029B9-FC95-4B69-B4A7-6B434C713E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Subcategoria</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>paangudi3@gmail.com</t>
+  </si>
+  <si>
+    <t>MetodoEntregaProducto</t>
+  </si>
+  <si>
+    <t>Recoge_en_tienda</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,9 +404,10 @@
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -410,8 +417,11 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -420,6 +430,9 @@
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
configuración de la ventana emergente método de entrega
</commit_message>
<xml_diff>
--- a/parametros/Datos.xlsx
+++ b/parametros/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semillero QA\projects\clickShop-automation\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF029B9-FC95-4B69-B4A7-6B434C713E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF1E7DB-D290-44E2-BF5B-33A1C8B56321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Subcategoria</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>paangudi3@gmail.com</t>
-  </si>
-  <si>
-    <t>MetodoEntregaProducto</t>
-  </si>
-  <si>
-    <t>Recoge_en_tienda</t>
   </si>
 </sst>
 </file>
@@ -393,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +401,7 @@
     <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,11 +411,8 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -430,9 +421,6 @@
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>